<commit_message>
GEO excel I-O fix
Found another typo in 'used' column for GEO vessels
</commit_message>
<xml_diff>
--- a/data_inputs/Inside_Park_Tables/GEOGRAPHE_202201_GEO_inside-outside_park_TL10_parkdist2128.xlsx
+++ b/data_inputs/Inside_Park_Tables/GEOGRAPHE_202201_GEO_inside-outside_park_TL10_parkdist2128.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -1867,8 +1867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T391"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="H80" sqref="H80"/>
+    <sheetView tabSelected="1" topLeftCell="A358" workbookViewId="0">
+      <selection activeCell="C376" sqref="C376"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16836,7 +16836,7 @@
         <v>1</v>
       </c>
       <c r="H254" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I254" s="2">
         <v>0</v>
@@ -24837,7 +24837,7 @@
     <row r="391" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H391">
         <f>SUM(H2:H389)</f>
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>